<commit_message>
added some polygon styles.
</commit_message>
<xml_diff>
--- a/doc/MIG-Annex-F-MOR-List-v3.1.14.xlsx
+++ b/doc/MIG-Annex-F-MOR-List-v3.1.14.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dehmer/Development/syncpoint.io/odin/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dehmer/Development/syncpoint.io/odin/openlayers/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91CACB0-4A4C-884A-BFC2-952A86FEB3C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401376BD-40C1-ED42-85FD-345B8825B3E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{06C7698E-B7EB-F34B-83A5-94075FAFE53B}"/>
+    <workbookView xWindow="14540" yWindow="460" windowWidth="36660" windowHeight="28340" xr2:uid="{06C7698E-B7EB-F34B-83A5-94075FAFE53B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="1309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="1311">
   <si>
     <t>1.X.2</t>
   </si>
@@ -3952,13 +3952,19 @@
   </si>
   <si>
     <t>EWX---</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>NO MAPPING AVAILABLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4038,13 +4044,25 @@
       <name val="Anonymous Pro"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -4059,7 +4077,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4126,6 +4144,13 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4442,11 +4467,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6EA0FD-3B04-734A-B049-07FEB6596675}">
   <dimension ref="A1:I270"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -4455,10 +4480,11 @@
     <col min="5" max="5" width="7.33203125" style="33" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="28" customFormat="1" ht="15">
       <c r="A1" s="26"/>
       <c r="B1" s="26" t="s">
         <v>248</v>
@@ -4476,8 +4502,11 @@
       <c r="G1" s="26" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="26" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
         <v>752</v>
       </c>
@@ -4500,7 +4529,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
         <v>753</v>
       </c>
@@ -4523,7 +4552,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
         <v>754</v>
       </c>
@@ -4546,7 +4575,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
         <v>755</v>
       </c>
@@ -4569,7 +4598,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
         <v>756</v>
       </c>
@@ -4592,7 +4621,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="6" t="s">
         <v>757</v>
       </c>
@@ -4615,7 +4644,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="6" t="s">
         <v>758</v>
       </c>
@@ -4638,7 +4667,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="6" t="s">
         <v>759</v>
       </c>
@@ -4661,7 +4690,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="6" t="s">
         <v>760</v>
       </c>
@@ -4684,7 +4713,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="6" t="s">
         <v>761</v>
       </c>
@@ -4707,7 +4736,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="6" t="s">
         <v>762</v>
       </c>
@@ -4730,7 +4759,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="6" t="s">
         <v>763</v>
       </c>
@@ -4753,7 +4782,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
         <v>764</v>
       </c>
@@ -4776,7 +4805,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="6" t="s">
         <v>765</v>
       </c>
@@ -4799,7 +4828,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
         <v>766</v>
       </c>
@@ -4822,7 +4851,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="6" t="s">
         <v>767</v>
       </c>
@@ -4845,7 +4874,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
         <v>768</v>
       </c>
@@ -4868,7 +4897,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
         <v>769</v>
       </c>
@@ -4891,7 +4920,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="6" t="s">
         <v>770</v>
       </c>
@@ -4914,7 +4943,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="6" t="s">
         <v>771</v>
       </c>
@@ -4937,7 +4966,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="6" t="s">
         <v>772</v>
       </c>
@@ -4960,7 +4989,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="6" t="s">
         <v>773</v>
       </c>
@@ -4983,7 +5012,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="6" t="s">
         <v>774</v>
       </c>
@@ -5006,7 +5035,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="6" t="s">
         <v>775</v>
       </c>
@@ -5029,7 +5058,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="6" t="s">
         <v>776</v>
       </c>
@@ -5052,7 +5081,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="6" t="s">
         <v>777</v>
       </c>
@@ -5075,7 +5104,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" s="6" t="s">
         <v>778</v>
       </c>
@@ -5098,7 +5127,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" s="6" t="s">
         <v>779</v>
       </c>
@@ -5121,7 +5150,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" s="6" t="s">
         <v>780</v>
       </c>
@@ -5144,7 +5173,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" s="6" t="s">
         <v>781</v>
       </c>
@@ -5167,7 +5196,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" s="6" t="s">
         <v>782</v>
       </c>
@@ -5190,7 +5219,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="6" t="s">
         <v>783</v>
       </c>
@@ -5213,7 +5242,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="6" t="s">
         <v>784</v>
       </c>
@@ -5236,7 +5265,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="6" t="s">
         <v>785</v>
       </c>
@@ -5259,7 +5288,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="6" t="s">
         <v>786</v>
       </c>
@@ -5282,7 +5311,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="6" t="s">
         <v>787</v>
       </c>
@@ -5305,7 +5334,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="6" t="s">
         <v>788</v>
       </c>
@@ -5328,7 +5357,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="6" t="s">
         <v>789</v>
       </c>
@@ -5351,7 +5380,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="6" t="s">
         <v>790</v>
       </c>
@@ -5374,7 +5403,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="6" t="s">
         <v>791</v>
       </c>
@@ -5397,7 +5426,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="6" t="s">
         <v>792</v>
       </c>
@@ -5420,7 +5449,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="6" t="s">
         <v>793</v>
       </c>
@@ -5443,7 +5472,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="6" t="s">
         <v>794</v>
       </c>
@@ -5466,7 +5495,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="6" t="s">
         <v>795</v>
       </c>
@@ -5489,7 +5518,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="6" t="s">
         <v>796</v>
       </c>
@@ -5512,7 +5541,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="6" t="s">
         <v>797</v>
       </c>
@@ -5533,7 +5562,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="6" t="s">
         <v>798</v>
       </c>
@@ -5554,7 +5583,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" s="6" t="s">
         <v>799</v>
       </c>
@@ -5577,7 +5606,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" s="6" t="s">
         <v>800</v>
       </c>
@@ -5600,7 +5629,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="A51" s="6" t="s">
         <v>801</v>
       </c>
@@ -5623,7 +5652,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" s="6" t="s">
         <v>802</v>
       </c>
@@ -5646,7 +5675,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="A53" s="6" t="s">
         <v>803</v>
       </c>
@@ -5669,7 +5698,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" s="6" t="s">
         <v>804</v>
       </c>
@@ -5692,7 +5721,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" s="6" t="s">
         <v>805</v>
       </c>
@@ -5715,7 +5744,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" s="6" t="s">
         <v>806</v>
       </c>
@@ -5738,7 +5767,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" s="6" t="s">
         <v>807</v>
       </c>
@@ -5761,7 +5790,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" s="6" t="s">
         <v>808</v>
       </c>
@@ -5784,7 +5813,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" s="6" t="s">
         <v>809</v>
       </c>
@@ -5807,7 +5836,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" s="6" t="s">
         <v>810</v>
       </c>
@@ -5830,7 +5859,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" s="6" t="s">
         <v>811</v>
       </c>
@@ -5853,7 +5882,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="A62" s="6" t="s">
         <v>812</v>
       </c>
@@ -5876,7 +5905,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="A63" s="6" t="s">
         <v>813</v>
       </c>
@@ -5899,7 +5928,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="A64" s="6" t="s">
         <v>814</v>
       </c>
@@ -5922,7 +5951,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" s="6" t="s">
         <v>815</v>
       </c>
@@ -5945,7 +5974,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" s="6" t="s">
         <v>816</v>
       </c>
@@ -5968,7 +5997,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7">
       <c r="A67" s="6" t="s">
         <v>817</v>
       </c>
@@ -5991,7 +6020,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7">
       <c r="A68" s="6" t="s">
         <v>818</v>
       </c>
@@ -6014,7 +6043,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7">
       <c r="A69" s="6" t="s">
         <v>819</v>
       </c>
@@ -6037,7 +6066,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7">
       <c r="A70" s="6" t="s">
         <v>820</v>
       </c>
@@ -6060,7 +6089,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7">
       <c r="A71" s="6" t="s">
         <v>821</v>
       </c>
@@ -6083,7 +6112,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7">
       <c r="A72" s="6" t="s">
         <v>822</v>
       </c>
@@ -6106,7 +6135,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7">
       <c r="A73" s="6" t="s">
         <v>823</v>
       </c>
@@ -6129,7 +6158,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7">
       <c r="A74" s="6" t="s">
         <v>824</v>
       </c>
@@ -6152,7 +6181,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7">
       <c r="A75" s="6" t="s">
         <v>825</v>
       </c>
@@ -6175,7 +6204,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7">
       <c r="A76" s="6" t="s">
         <v>826</v>
       </c>
@@ -6198,7 +6227,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7">
       <c r="A77" s="6" t="s">
         <v>827</v>
       </c>
@@ -6221,7 +6250,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7">
       <c r="A78" s="6" t="s">
         <v>828</v>
       </c>
@@ -6244,7 +6273,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7">
       <c r="A79" s="6" t="s">
         <v>829</v>
       </c>
@@ -6267,7 +6296,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80" s="6" t="s">
         <v>830</v>
       </c>
@@ -6290,7 +6319,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9">
       <c r="A81" s="6" t="s">
         <v>831</v>
       </c>
@@ -6313,7 +6342,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9">
       <c r="A82" s="6" t="s">
         <v>832</v>
       </c>
@@ -6336,7 +6365,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9">
       <c r="A83" s="6" t="s">
         <v>833</v>
       </c>
@@ -6359,7 +6388,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="84" spans="1:9" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" s="3" customFormat="1" ht="15">
       <c r="A84" s="9" t="s">
         <v>834</v>
       </c>
@@ -6384,7 +6413,7 @@
       <c r="H84" s="36"/>
       <c r="I84" s="36"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9">
       <c r="A85" s="6" t="s">
         <v>835</v>
       </c>
@@ -6407,7 +6436,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9">
       <c r="A86" s="6" t="s">
         <v>836</v>
       </c>
@@ -6430,7 +6459,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9">
       <c r="A87" s="6" t="s">
         <v>837</v>
       </c>
@@ -6453,7 +6482,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9">
       <c r="A88" s="6" t="s">
         <v>838</v>
       </c>
@@ -6476,7 +6505,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9">
       <c r="A89" s="6" t="s">
         <v>839</v>
       </c>
@@ -6499,7 +6528,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9">
       <c r="A90" s="6" t="s">
         <v>840</v>
       </c>
@@ -6522,7 +6551,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9">
       <c r="A91" s="6" t="s">
         <v>841</v>
       </c>
@@ -6545,7 +6574,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9">
       <c r="A92" s="6" t="s">
         <v>842</v>
       </c>
@@ -6568,7 +6597,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9">
       <c r="A93" s="6" t="s">
         <v>843</v>
       </c>
@@ -6591,7 +6620,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9">
       <c r="A94" s="6" t="s">
         <v>844</v>
       </c>
@@ -6614,7 +6643,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9">
       <c r="A95" s="6" t="s">
         <v>845</v>
       </c>
@@ -6637,7 +6666,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9">
       <c r="A96" s="6" t="s">
         <v>846</v>
       </c>
@@ -6660,7 +6689,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7">
       <c r="A97" s="6" t="s">
         <v>847</v>
       </c>
@@ -6683,7 +6712,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7">
       <c r="A98" s="6" t="s">
         <v>848</v>
       </c>
@@ -6706,7 +6735,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" s="23" customFormat="1">
       <c r="A99" s="19" t="s">
         <v>849</v>
       </c>
@@ -6727,7 +6756,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="15">
       <c r="A100" s="6" t="s">
         <v>850</v>
       </c>
@@ -6750,7 +6779,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7">
       <c r="A101" s="6" t="s">
         <v>851</v>
       </c>
@@ -6773,7 +6802,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" s="23" customFormat="1">
       <c r="A102" s="19" t="s">
         <v>852</v>
       </c>
@@ -6794,7 +6823,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7">
       <c r="A103" s="6" t="s">
         <v>853</v>
       </c>
@@ -6817,7 +6846,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7">
       <c r="A104" s="6" t="s">
         <v>854</v>
       </c>
@@ -6840,7 +6869,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7">
       <c r="A105" s="6" t="s">
         <v>855</v>
       </c>
@@ -6863,7 +6892,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7">
       <c r="A106" s="6" t="s">
         <v>856</v>
       </c>
@@ -6886,7 +6915,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7">
       <c r="A107" s="6" t="s">
         <v>857</v>
       </c>
@@ -6909,7 +6938,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7">
       <c r="A108" s="6" t="s">
         <v>858</v>
       </c>
@@ -6932,7 +6961,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7">
       <c r="A109" s="6" t="s">
         <v>859</v>
       </c>
@@ -6955,7 +6984,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7">
       <c r="A110" s="6" t="s">
         <v>860</v>
       </c>
@@ -6978,7 +7007,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7">
       <c r="A111" s="6" t="s">
         <v>861</v>
       </c>
@@ -7001,7 +7030,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7">
       <c r="A112" s="6" t="s">
         <v>862</v>
       </c>
@@ -7024,7 +7053,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7">
       <c r="A113" s="6" t="s">
         <v>863</v>
       </c>
@@ -7047,7 +7076,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7">
       <c r="A114" s="6" t="s">
         <v>864</v>
       </c>
@@ -7070,7 +7099,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7">
       <c r="A115" s="6" t="s">
         <v>865</v>
       </c>
@@ -7093,7 +7122,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7">
       <c r="A116" s="6" t="s">
         <v>866</v>
       </c>
@@ -7116,7 +7145,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7">
       <c r="A117" s="6" t="s">
         <v>867</v>
       </c>
@@ -7139,7 +7168,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7">
       <c r="A118" s="6" t="s">
         <v>868</v>
       </c>
@@ -7162,7 +7191,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7">
       <c r="A119" s="6" t="s">
         <v>869</v>
       </c>
@@ -7185,7 +7214,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7">
       <c r="A120" s="6" t="s">
         <v>870</v>
       </c>
@@ -7208,7 +7237,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7">
       <c r="A121" s="6" t="s">
         <v>871</v>
       </c>
@@ -7231,7 +7260,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7">
       <c r="A122" s="6" t="s">
         <v>872</v>
       </c>
@@ -7254,7 +7283,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7">
       <c r="A123" s="6" t="s">
         <v>873</v>
       </c>
@@ -7277,7 +7306,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7">
       <c r="A124" s="6" t="s">
         <v>874</v>
       </c>
@@ -7300,7 +7329,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7">
       <c r="A125" s="6" t="s">
         <v>875</v>
       </c>
@@ -7323,7 +7352,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7">
       <c r="A126" s="6" t="s">
         <v>876</v>
       </c>
@@ -7346,7 +7375,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7">
       <c r="A127" s="6" t="s">
         <v>877</v>
       </c>
@@ -7369,7 +7398,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7">
       <c r="A128" s="6" t="s">
         <v>878</v>
       </c>
@@ -7392,7 +7421,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8">
       <c r="A129" s="6" t="s">
         <v>879</v>
       </c>
@@ -7415,7 +7444,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="130" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" s="23" customFormat="1">
       <c r="A130" s="19" t="s">
         <v>880</v>
       </c>
@@ -7436,7 +7465,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" ht="15">
       <c r="A131" s="6" t="s">
         <v>881</v>
       </c>
@@ -7459,7 +7488,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8">
       <c r="A132" s="6" t="s">
         <v>882</v>
       </c>
@@ -7482,30 +7511,33 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A133" s="6" t="s">
+    <row r="133" spans="1:8" s="38" customFormat="1">
+      <c r="A133" s="39" t="s">
         <v>883</v>
       </c>
-      <c r="B133" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="C133" s="16" t="s">
+      <c r="B133" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="C133" s="41" t="s">
         <v>540</v>
       </c>
-      <c r="D133" s="24" t="s">
+      <c r="D133" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="E133" s="29" t="s">
+      <c r="E133" s="42" t="s">
         <v>589</v>
       </c>
-      <c r="F133" s="4" t="s">
+      <c r="F133" s="40" t="s">
         <v>588</v>
       </c>
-      <c r="G133" s="4" t="s">
+      <c r="G133" s="40" t="s">
         <v>1160</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H133" s="40" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
       <c r="A134" s="6" t="s">
         <v>884</v>
       </c>
@@ -7528,7 +7560,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8">
       <c r="A135" s="6" t="s">
         <v>885</v>
       </c>
@@ -7551,7 +7583,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8">
       <c r="A136" s="6" t="s">
         <v>886</v>
       </c>
@@ -7574,7 +7606,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8">
       <c r="A137" s="6" t="s">
         <v>887</v>
       </c>
@@ -7597,7 +7629,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8">
       <c r="A138" s="6" t="s">
         <v>888</v>
       </c>
@@ -7620,7 +7652,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8">
       <c r="A139" s="6" t="s">
         <v>889</v>
       </c>
@@ -7643,7 +7675,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8">
       <c r="A140" s="6" t="s">
         <v>890</v>
       </c>
@@ -7666,7 +7698,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8">
       <c r="A141" s="6" t="s">
         <v>891</v>
       </c>
@@ -7689,7 +7721,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8">
       <c r="A142" s="6" t="s">
         <v>892</v>
       </c>
@@ -7712,7 +7744,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8">
       <c r="A143" s="6" t="s">
         <v>893</v>
       </c>
@@ -7735,7 +7767,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8">
       <c r="A144" s="6" t="s">
         <v>894</v>
       </c>
@@ -7758,7 +7790,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7">
       <c r="A145" s="6" t="s">
         <v>895</v>
       </c>
@@ -7781,7 +7813,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7">
       <c r="A146" s="6" t="s">
         <v>896</v>
       </c>
@@ -7804,7 +7836,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7">
       <c r="A147" s="6" t="s">
         <v>897</v>
       </c>
@@ -7827,7 +7859,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7">
       <c r="A148" s="6" t="s">
         <v>898</v>
       </c>
@@ -7850,7 +7882,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7">
       <c r="A149" s="6" t="s">
         <v>899</v>
       </c>
@@ -7873,7 +7905,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7">
       <c r="A150" s="6" t="s">
         <v>900</v>
       </c>
@@ -7896,7 +7928,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7">
       <c r="A151" s="6" t="s">
         <v>901</v>
       </c>
@@ -7919,7 +7951,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7">
       <c r="A152" s="6" t="s">
         <v>902</v>
       </c>
@@ -7942,7 +7974,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7">
       <c r="A153" s="6" t="s">
         <v>903</v>
       </c>
@@ -7965,7 +7997,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7">
       <c r="A154" s="6" t="s">
         <v>904</v>
       </c>
@@ -7988,7 +8020,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7">
       <c r="A155" s="6" t="s">
         <v>905</v>
       </c>
@@ -8011,7 +8043,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7">
       <c r="A156" s="6" t="s">
         <v>906</v>
       </c>
@@ -8034,7 +8066,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7">
       <c r="A157" s="6" t="s">
         <v>907</v>
       </c>
@@ -8057,7 +8089,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7">
       <c r="A158" s="6" t="s">
         <v>908</v>
       </c>
@@ -8080,7 +8112,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7">
       <c r="A159" s="6" t="s">
         <v>909</v>
       </c>
@@ -8103,7 +8135,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7">
       <c r="A160" s="6" t="s">
         <v>910</v>
       </c>
@@ -8126,7 +8158,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7">
       <c r="A161" s="6" t="s">
         <v>911</v>
       </c>
@@ -8149,7 +8181,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7">
       <c r="A162" s="6" t="s">
         <v>912</v>
       </c>
@@ -8172,7 +8204,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7">
       <c r="A163" s="6" t="s">
         <v>913</v>
       </c>
@@ -8195,7 +8227,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7">
       <c r="A164" s="6" t="s">
         <v>914</v>
       </c>
@@ -8218,7 +8250,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7">
       <c r="A165" s="6" t="s">
         <v>915</v>
       </c>
@@ -8241,7 +8273,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7">
       <c r="A166" s="6" t="s">
         <v>916</v>
       </c>
@@ -8264,7 +8296,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7">
       <c r="A167" s="6" t="s">
         <v>917</v>
       </c>
@@ -8287,7 +8319,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" ht="15">
       <c r="A168" s="6" t="s">
         <v>918</v>
       </c>
@@ -8310,7 +8342,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7">
       <c r="A169" s="6" t="s">
         <v>919</v>
       </c>
@@ -8333,7 +8365,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7">
       <c r="A170" s="6" t="s">
         <v>920</v>
       </c>
@@ -8356,7 +8388,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7">
       <c r="A171" s="6" t="s">
         <v>921</v>
       </c>
@@ -8379,7 +8411,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7">
       <c r="A172" s="6" t="s">
         <v>922</v>
       </c>
@@ -8402,7 +8434,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7">
       <c r="A173" s="6" t="s">
         <v>923</v>
       </c>
@@ -8425,7 +8457,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7">
       <c r="A174" s="6" t="s">
         <v>924</v>
       </c>
@@ -8448,7 +8480,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7">
       <c r="A175" s="6" t="s">
         <v>925</v>
       </c>
@@ -8471,7 +8503,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7">
       <c r="A176" s="6" t="s">
         <v>926</v>
       </c>
@@ -8494,7 +8526,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7">
       <c r="A177" s="6" t="s">
         <v>927</v>
       </c>
@@ -8517,7 +8549,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7">
       <c r="A178" s="6" t="s">
         <v>928</v>
       </c>
@@ -8540,7 +8572,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7">
       <c r="A179" s="6" t="s">
         <v>929</v>
       </c>
@@ -8563,7 +8595,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7">
       <c r="A180" s="6" t="s">
         <v>930</v>
       </c>
@@ -8586,7 +8618,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7">
       <c r="A181" s="6" t="s">
         <v>931</v>
       </c>
@@ -8609,7 +8641,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7">
       <c r="A182" s="6" t="s">
         <v>932</v>
       </c>
@@ -8632,7 +8664,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7">
       <c r="A183" s="6" t="s">
         <v>933</v>
       </c>
@@ -8655,7 +8687,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7">
       <c r="A184" s="6" t="s">
         <v>934</v>
       </c>
@@ -8678,7 +8710,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7">
       <c r="A185" s="6" t="s">
         <v>935</v>
       </c>
@@ -8701,7 +8733,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7">
       <c r="A186" s="6" t="s">
         <v>936</v>
       </c>
@@ -8724,7 +8756,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7">
       <c r="A187" s="6" t="s">
         <v>937</v>
       </c>
@@ -8747,7 +8779,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" ht="15">
       <c r="A188" s="6" t="s">
         <v>938</v>
       </c>
@@ -8770,7 +8802,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7">
       <c r="A189" s="6" t="s">
         <v>939</v>
       </c>
@@ -8793,7 +8825,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7">
       <c r="A190" s="6" t="s">
         <v>940</v>
       </c>
@@ -8816,7 +8848,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7">
       <c r="A191" s="6" t="s">
         <v>941</v>
       </c>
@@ -8839,7 +8871,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7">
       <c r="A192" s="6" t="s">
         <v>942</v>
       </c>
@@ -8862,7 +8894,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7">
       <c r="A193" s="6" t="s">
         <v>943</v>
       </c>
@@ -8885,7 +8917,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7">
       <c r="A194" s="6" t="s">
         <v>944</v>
       </c>
@@ -8908,7 +8940,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7">
       <c r="A195" s="6" t="s">
         <v>945</v>
       </c>
@@ -8931,7 +8963,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7">
       <c r="A196" s="6" t="s">
         <v>946</v>
       </c>
@@ -8954,7 +8986,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7">
       <c r="A197" s="6" t="s">
         <v>947</v>
       </c>
@@ -8977,7 +9009,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7">
       <c r="A198" s="6" t="s">
         <v>948</v>
       </c>
@@ -9000,7 +9032,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7">
       <c r="A199" s="6" t="s">
         <v>949</v>
       </c>
@@ -9023,7 +9055,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7">
       <c r="A200" s="6" t="s">
         <v>950</v>
       </c>
@@ -9046,7 +9078,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7">
       <c r="A201" s="6" t="s">
         <v>951</v>
       </c>
@@ -9067,7 +9099,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7">
       <c r="A202" s="6" t="s">
         <v>952</v>
       </c>
@@ -9088,7 +9120,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7">
       <c r="A203" s="6" t="s">
         <v>953</v>
       </c>
@@ -9111,7 +9143,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7">
       <c r="A204" s="6" t="s">
         <v>954</v>
       </c>
@@ -9134,7 +9166,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7">
       <c r="A205" s="6" t="s">
         <v>955</v>
       </c>
@@ -9157,7 +9189,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7">
       <c r="A206" s="6" t="s">
         <v>956</v>
       </c>
@@ -9180,7 +9212,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7">
       <c r="A207" s="6" t="s">
         <v>957</v>
       </c>
@@ -9203,7 +9235,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7">
       <c r="A208" s="6" t="s">
         <v>958</v>
       </c>
@@ -9226,7 +9258,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7">
       <c r="A209" s="6" t="s">
         <v>959</v>
       </c>
@@ -9249,7 +9281,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7">
       <c r="A210" s="6" t="s">
         <v>960</v>
       </c>
@@ -9272,7 +9304,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7">
       <c r="A211" s="6" t="s">
         <v>961</v>
       </c>
@@ -9295,7 +9327,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7">
       <c r="A212" s="6" t="s">
         <v>962</v>
       </c>
@@ -9318,7 +9350,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7">
       <c r="A213" s="6" t="s">
         <v>963</v>
       </c>
@@ -9341,7 +9373,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7">
       <c r="A214" s="6" t="s">
         <v>964</v>
       </c>
@@ -9364,7 +9396,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7">
       <c r="A215" s="6" t="s">
         <v>965</v>
       </c>
@@ -9387,7 +9419,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7">
       <c r="A216" s="6" t="s">
         <v>966</v>
       </c>
@@ -9410,7 +9442,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7">
       <c r="A217" s="6" t="s">
         <v>967</v>
       </c>
@@ -9433,7 +9465,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7">
       <c r="A218" s="6" t="s">
         <v>968</v>
       </c>
@@ -9456,7 +9488,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7">
       <c r="A219" s="6" t="s">
         <v>969</v>
       </c>
@@ -9477,7 +9509,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7" ht="15">
       <c r="A220" s="6" t="s">
         <v>970</v>
       </c>
@@ -9500,7 +9532,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" ht="15">
       <c r="A221" s="6" t="s">
         <v>971</v>
       </c>
@@ -9523,7 +9555,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7">
       <c r="A222" s="6" t="s">
         <v>972</v>
       </c>
@@ -9535,7 +9567,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7" ht="15">
       <c r="A223" s="6" t="s">
         <v>973</v>
       </c>
@@ -9558,7 +9590,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:7">
       <c r="A224" s="6" t="s">
         <v>974</v>
       </c>
@@ -9581,7 +9613,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" ht="15">
       <c r="A225" s="6" t="s">
         <v>975</v>
       </c>
@@ -9604,7 +9636,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7">
       <c r="A226" s="6" t="s">
         <v>976</v>
       </c>
@@ -9627,7 +9659,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7">
       <c r="A227" s="6" t="s">
         <v>977</v>
       </c>
@@ -9650,7 +9682,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7">
       <c r="A228" s="6" t="s">
         <v>978</v>
       </c>
@@ -9671,7 +9703,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7">
       <c r="A229" s="6" t="s">
         <v>979</v>
       </c>
@@ -9692,7 +9724,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:7">
       <c r="A230" s="6" t="s">
         <v>980</v>
       </c>
@@ -9713,7 +9745,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7">
       <c r="A231" s="6" t="s">
         <v>981</v>
       </c>
@@ -9736,7 +9768,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:7">
       <c r="A232" s="6" t="s">
         <v>982</v>
       </c>
@@ -9759,7 +9791,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:7">
       <c r="A233" s="6" t="s">
         <v>983</v>
       </c>
@@ -9782,7 +9814,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:7">
       <c r="A234" s="6" t="s">
         <v>984</v>
       </c>
@@ -9805,7 +9837,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:7">
       <c r="A235" s="6" t="s">
         <v>985</v>
       </c>
@@ -9828,7 +9860,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:7">
       <c r="A236" s="6" t="s">
         <v>986</v>
       </c>
@@ -9851,7 +9883,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:7">
       <c r="A237" s="6" t="s">
         <v>987</v>
       </c>
@@ -9874,7 +9906,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7">
       <c r="A238" s="6" t="s">
         <v>988</v>
       </c>
@@ -9897,7 +9929,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7">
       <c r="A239" s="6" t="s">
         <v>989</v>
       </c>
@@ -9920,7 +9952,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7">
       <c r="A240" s="6" t="s">
         <v>990</v>
       </c>
@@ -9943,7 +9975,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:7">
       <c r="A241" s="6" t="s">
         <v>991</v>
       </c>
@@ -9964,7 +9996,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:7">
       <c r="A242" s="6" t="s">
         <v>992</v>
       </c>
@@ -9987,7 +10019,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:7">
       <c r="A243" s="6" t="s">
         <v>993</v>
       </c>
@@ -10010,7 +10042,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:7">
       <c r="A244" s="6" t="s">
         <v>994</v>
       </c>
@@ -10033,7 +10065,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:7">
       <c r="A245" s="6" t="s">
         <v>995</v>
       </c>
@@ -10056,7 +10088,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:7">
       <c r="A246" s="6" t="s">
         <v>996</v>
       </c>
@@ -10079,7 +10111,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:7">
       <c r="A247" s="6" t="s">
         <v>997</v>
       </c>
@@ -10102,7 +10134,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:7">
       <c r="A248" s="6" t="s">
         <v>998</v>
       </c>
@@ -10125,7 +10157,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:7">
       <c r="A249" s="6" t="s">
         <v>999</v>
       </c>
@@ -10146,7 +10178,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:7">
       <c r="A250" s="6" t="s">
         <v>1000</v>
       </c>
@@ -10167,7 +10199,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:7">
       <c r="A251" s="6" t="s">
         <v>1001</v>
       </c>
@@ -10190,7 +10222,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:7">
       <c r="A252" s="6" t="s">
         <v>1002</v>
       </c>
@@ -10211,7 +10243,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:7">
       <c r="A253" s="6" t="s">
         <v>1003</v>
       </c>
@@ -10232,7 +10264,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:7">
       <c r="A254" s="6" t="s">
         <v>1004</v>
       </c>
@@ -10255,7 +10287,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:7">
       <c r="A255" s="6" t="s">
         <v>1005</v>
       </c>
@@ -10278,7 +10310,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:7">
       <c r="A256" s="6" t="s">
         <v>1006</v>
       </c>
@@ -10301,7 +10333,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:7">
       <c r="A257" s="6" t="s">
         <v>1007</v>
       </c>
@@ -10324,7 +10356,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:7">
       <c r="A258" s="6" t="s">
         <v>1008</v>
       </c>
@@ -10347,7 +10379,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7">
       <c r="A259" s="6" t="s">
         <v>1009</v>
       </c>
@@ -10370,7 +10402,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:7">
       <c r="A260" s="6" t="s">
         <v>1010</v>
       </c>
@@ -10393,7 +10425,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:7">
       <c r="A261" s="6" t="s">
         <v>1011</v>
       </c>
@@ -10416,7 +10448,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:7">
       <c r="A262" s="6" t="s">
         <v>1012</v>
       </c>
@@ -10439,7 +10471,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:7">
       <c r="A263" s="6" t="s">
         <v>1013</v>
       </c>
@@ -10462,7 +10494,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:7">
       <c r="A264" s="6" t="s">
         <v>1014</v>
       </c>
@@ -10485,7 +10517,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:7">
       <c r="A265" s="6" t="s">
         <v>1015</v>
       </c>
@@ -10508,7 +10540,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:7">
       <c r="A266" s="6" t="s">
         <v>1016</v>
       </c>
@@ -10531,7 +10563,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:7">
       <c r="A267" s="6" t="s">
         <v>1017</v>
       </c>
@@ -10552,7 +10584,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:7">
       <c r="A268" s="6" t="s">
         <v>1018</v>
       </c>
@@ -10575,7 +10607,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:7">
       <c r="A269" s="6" t="s">
         <v>1019</v>
       </c>
@@ -10598,7 +10630,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:7">
       <c r="A270" s="6" t="s">
         <v>1020</v>
       </c>

</xml_diff>